<commit_message>
custom peiir and rtmf (request from ben)
</commit_message>
<xml_diff>
--- a/InputData/fuels/PEIIR/Pollutant Emissions Intensity Improvement Rate.xlsx
+++ b/InputData/fuels/PEIIR/Pollutant Emissions Intensity Improvement Rate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\fuels\PEIIR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Rhode Island\RI-eps\InputData\fuels\PEIIR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C5BDB8-164C-4260-8BDD-310BFE54C72D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5D80E2-0A78-4EE9-BDC3-E6D88891A366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21045" yWindow="1410" windowWidth="33360" windowHeight="21225" tabRatio="783" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="19200" windowHeight="10060" tabRatio="783" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -328,23 +328,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -701,133 +694,133 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
     <col min="2" max="2" width="73" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -847,55 +840,55 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" customWidth="1"/>
+    <col min="9" max="9" width="15.26953125" customWidth="1"/>
+    <col min="10" max="10" width="13.54296875" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -930,7 +923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -965,7 +958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1000,7 +993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1035,7 +1028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1070,7 +1063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1105,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1140,7 +1133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1175,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1210,7 +1203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1245,7 +1238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1280,7 +1273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1330,56 +1323,56 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1414,7 +1407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1449,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1484,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1519,7 +1512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1554,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1589,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1624,7 +1617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1659,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1694,7 +1687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1729,7 +1722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1764,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1814,22 +1807,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1850,20 +1843,20 @@
       <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1898,7 +1891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1933,7 +1926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1968,7 +1961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2003,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2038,7 +2031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2073,7 +2066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2108,7 +2101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2143,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2178,7 +2171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2213,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2248,7 +2241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2298,56 +2291,56 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2382,7 +2375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2417,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2452,7 +2445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2487,7 +2480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2522,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2557,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2592,7 +2585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2627,7 +2620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2662,7 +2655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2697,7 +2690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2732,7 +2725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2782,56 +2775,56 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2866,7 +2859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2901,7 +2894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2936,7 +2929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2971,7 +2964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3006,7 +2999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3041,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3076,7 +3069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3111,7 +3104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3146,7 +3139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3181,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3216,7 +3209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -3266,28 +3259,28 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -3296,26 +3289,26 @@
       <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3350,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3385,7 +3378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3420,7 +3413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3455,7 +3448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3490,7 +3483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3525,7 +3518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3560,7 +3553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3595,7 +3588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3630,7 +3623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3665,7 +3658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3700,7 +3693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -3750,31 +3743,31 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -3786,20 +3779,20 @@
       <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3834,7 +3827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3869,7 +3862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3904,7 +3897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3939,7 +3932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3974,7 +3967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4009,7 +4002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4044,7 +4037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4079,7 +4072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4114,7 +4107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -4149,7 +4142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -4184,7 +4177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -4234,78 +4227,78 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7265625" customWidth="1"/>
+    <col min="10" max="10" width="15.7265625" customWidth="1"/>
+    <col min="11" max="11" width="16.1796875" customWidth="1"/>
+    <col min="12" max="12" width="20.7265625" customWidth="1"/>
+    <col min="13" max="13" width="13.7265625" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1796875" customWidth="1"/>
+    <col min="16" max="16" width="17.1796875" customWidth="1"/>
+    <col min="17" max="17" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4358,7 +4351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4411,7 +4404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4464,7 +4457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4517,7 +4510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4570,7 +4563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4623,7 +4616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4676,7 +4669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4729,7 +4722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4782,7 +4775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -4835,7 +4828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -4888,7 +4881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -4954,23 +4947,25 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" customWidth="1"/>
+    <col min="9" max="9" width="24.7265625" customWidth="1"/>
+    <col min="10" max="10" width="22.81640625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -5004,7 +4999,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5018,7 +5013,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -5030,7 +5025,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -5039,7 +5034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -5074,7 +5069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5109,7 +5104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -5144,7 +5139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -5179,7 +5174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -5214,7 +5209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -5249,7 +5244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5284,7 +5279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -5319,7 +5314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -5354,7 +5349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -5389,7 +5384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
take out rps and PEIIR
</commit_message>
<xml_diff>
--- a/InputData/fuels/PEIIR/Pollutant Emissions Intensity Improvement Rate.xlsx
+++ b/InputData/fuels/PEIIR/Pollutant Emissions Intensity Improvement Rate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Rhode Island\RI-eps\InputData\fuels\PEIIR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\fuels\PEIIR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5D80E2-0A78-4EE9-BDC3-E6D88891A366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C5BDB8-164C-4260-8BDD-310BFE54C72D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="19200" windowHeight="10060" tabRatio="783" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21045" yWindow="1410" windowWidth="33360" windowHeight="21225" tabRatio="783" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -328,16 +328,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -694,133 +701,133 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="73" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -840,55 +847,55 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" customWidth="1"/>
-    <col min="8" max="8" width="13.26953125" customWidth="1"/>
-    <col min="9" max="9" width="15.26953125" customWidth="1"/>
-    <col min="10" max="10" width="13.54296875" customWidth="1"/>
-    <col min="11" max="11" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -923,7 +930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -958,7 +965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -993,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1028,7 +1035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1063,7 +1070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1098,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1133,7 +1140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1168,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1203,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1238,7 +1245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1273,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1323,56 +1330,56 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" customWidth="1"/>
-    <col min="10" max="10" width="13.1796875" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1407,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1442,7 +1449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1477,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1512,7 +1519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1547,7 +1554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1582,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1617,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1652,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1687,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1722,7 +1729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1757,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1807,22 +1814,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" customWidth="1"/>
-    <col min="10" max="10" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1843,20 +1850,20 @@
       <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1891,7 +1898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1926,7 +1933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1961,7 +1968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1996,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2031,7 +2038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2066,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2101,7 +2108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2136,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2171,7 +2178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2206,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2241,7 +2248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2291,56 +2298,56 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" customWidth="1"/>
-    <col min="8" max="8" width="14.54296875" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" customWidth="1"/>
-    <col min="10" max="10" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>26</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2375,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2410,7 +2417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2445,7 +2452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2480,7 +2487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2515,7 +2522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2550,7 +2557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2585,7 +2592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2620,7 +2627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2655,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2690,7 +2697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2725,7 +2732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2775,56 +2782,56 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" customWidth="1"/>
-    <col min="10" max="10" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2859,7 +2866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2894,7 +2901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2929,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2964,7 +2971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2999,7 +3006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3034,7 +3041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3069,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3104,7 +3111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3139,7 +3146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3174,7 +3181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3209,7 +3216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -3259,28 +3266,28 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" customWidth="1"/>
-    <col min="10" max="10" width="13.1796875" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -3289,26 +3296,26 @@
       <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3343,7 +3350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3378,7 +3385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3413,7 +3420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3448,7 +3455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3483,7 +3490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3518,7 +3525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3553,7 +3560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3588,7 +3595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3623,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3658,7 +3665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3693,7 +3700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -3743,31 +3750,31 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" customWidth="1"/>
-    <col min="10" max="10" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -3779,20 +3786,20 @@
       <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3827,7 +3834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3862,7 +3869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3897,7 +3904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3932,7 +3939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3967,7 +3974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4002,7 +4009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4037,7 +4044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4072,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4107,7 +4114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -4142,7 +4149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -4177,7 +4184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -4227,78 +4234,78 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="12.7265625" customWidth="1"/>
-    <col min="10" max="10" width="15.7265625" customWidth="1"/>
-    <col min="11" max="11" width="16.1796875" customWidth="1"/>
-    <col min="12" max="12" width="20.7265625" customWidth="1"/>
-    <col min="13" max="13" width="13.7265625" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.1796875" customWidth="1"/>
-    <col min="16" max="16" width="17.1796875" customWidth="1"/>
-    <col min="17" max="17" width="15.54296875" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4351,7 +4358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4404,7 +4411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4457,7 +4464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4510,7 +4517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4563,7 +4570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4616,7 +4623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4669,7 +4676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4722,7 +4729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4775,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -4828,7 +4835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -4881,7 +4888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -4947,25 +4954,23 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.1796875" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="7" max="7" width="14.7265625" customWidth="1"/>
-    <col min="8" max="8" width="13.26953125" customWidth="1"/>
-    <col min="9" max="9" width="24.7265625" customWidth="1"/>
-    <col min="10" max="10" width="22.81640625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -4999,7 +5004,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5013,7 +5018,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -5025,7 +5030,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -5034,7 +5039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -5069,7 +5074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5104,7 +5109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -5139,7 +5144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -5174,7 +5179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -5209,7 +5214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -5244,7 +5249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5279,7 +5284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -5314,7 +5319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -5349,7 +5354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -5384,7 +5389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
biofuel and rps policy included
</commit_message>
<xml_diff>
--- a/InputData/fuels/PEIIR/Pollutant Emissions Intensity Improvement Rate.xlsx
+++ b/InputData/fuels/PEIIR/Pollutant Emissions Intensity Improvement Rate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\fuels\PEIIR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Rhode Island\RI-eps\InputData\fuels\PEIIR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C5BDB8-164C-4260-8BDD-310BFE54C72D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2CD53AC-8742-4568-8648-1943016ED6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21045" yWindow="1410" windowWidth="33360" windowHeight="21225" tabRatio="783" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="14850" windowHeight="13950" tabRatio="783" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -328,23 +328,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -701,7 +694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -733,7 +726,7 @@
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -860,38 +853,38 @@
     <col min="11" max="11" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1344,38 +1337,38 @@
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1829,7 +1822,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1850,16 +1843,16 @@
       <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2313,37 +2306,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2797,37 +2790,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3281,13 +3274,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -3296,22 +3289,22 @@
       <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3765,16 +3758,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -3786,16 +3779,16 @@
       <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -4252,56 +4245,56 @@
     <col min="17" max="17" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="4" t="s">
         <v>64</v>
       </c>
     </row>
@@ -4954,7 +4947,9 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4970,7 +4965,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -5018,7 +5013,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -5030,7 +5025,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="J2">
         <v>0</v>

</xml_diff>